<commit_message>
Div et perf fonctionnent a chaque test, probleme sur payoff
</commit_message>
<xml_diff>
--- a/Excel/casDefav.xlsx
+++ b/Excel/casDefav.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\3A\peps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\PEPSI\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190438F4-9705-4B2F-9834-60EDF68A7588}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAC31DE-881C-43F0-B281-3BDAD6979340}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7440" xr2:uid="{5172E695-FFD0-4A81-8853-8CB156196831}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="283">
   <si>
     <t>1215.38</t>
   </si>
@@ -878,6 +878,9 @@
   </si>
   <si>
     <t>1272.4</t>
+  </si>
+  <si>
+    <t>Moyenne des performances prenant en compte le point d'entrée</t>
   </si>
 </sst>
 </file>
@@ -1352,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8926E1A2-95A1-4361-8542-D3980DDE6A70}">
   <dimension ref="A1:AK88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC52" sqref="AC52"/>
+    <sheetView tabSelected="1" topLeftCell="T23" workbookViewId="0">
+      <selection activeCell="AF33" sqref="AF33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2522,111 +2525,111 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <f>(B4-B$3)/B$3</f>
-        <v>9.9999999999999811E-2</v>
+        <f>(B4)/B$3</f>
+        <v>1.0999999999999999</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="B19:Z19" si="0">(C4-C$3)/C$3</f>
-        <v>0.10000000000000005</v>
+        <f t="shared" ref="C19:Z22" si="0">(C4)/C$3</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000007</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0.1000000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>0.1000000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>0.14999999999999997</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000012</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000013</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000006</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
-        <v>6.0000000000000081E-2</v>
+        <v>1.06</v>
       </c>
       <c r="N19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000003</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O19">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="P19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000006</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
-        <v>7.9999999999999891E-2</v>
+        <v>1.0799999999999998</v>
       </c>
       <c r="R19">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000005</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T19">
         <f t="shared" si="0"/>
-        <v>0.25000002057961251</v>
+        <v>1.2500000205796125</v>
       </c>
       <c r="U19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000005</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V19">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="W19">
         <f t="shared" si="0"/>
-        <v>4.999999999999994E-2</v>
+        <v>1.05</v>
       </c>
       <c r="X19">
         <f t="shared" si="0"/>
-        <v>0.10000000000000014</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y19">
         <f t="shared" si="0"/>
-        <v>9.999999999999995E-2</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="Z19">
-        <f>(Z4-Z$3)/Z$3</f>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AB19">
         <f>AVERAGE(B19:Z19)</f>
-        <v>0.10360000082318453</v>
+        <v>1.1036000008231848</v>
       </c>
       <c r="AD19" s="7">
-        <f>MIN(0,AB19:AB22)+1</f>
+        <f>MIN(1,AB19:AB22)</f>
         <v>1</v>
       </c>
     </row>
@@ -2635,108 +2638,108 @@
         <v>2</v>
       </c>
       <c r="B20">
-        <f>(B5-B$3)/B$3</f>
-        <v>0.11999999999999988</v>
+        <f t="shared" ref="B20:Q22" si="1">(B5)/B$3</f>
+        <v>1.1199999999999999</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:Z20" si="1">(C5-C$3)/C$3</f>
-        <v>0.10000000000000005</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>0.16000000000000011</v>
+        <v>1.1600000000000001</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>0.11999999999999993</v>
+        <v>1.1199999999999999</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>0.1000000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>6.0000000000000026E-2</v>
+        <v>1.06</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>-2.0000000000000153E-2</v>
+        <v>0.97999999999999987</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>0.10000000000000012</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K20">
         <f t="shared" si="1"/>
-        <v>-4.9999999999999906E-2</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>0.10000000000000006</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>-6.9999999999999937E-2</v>
+        <v>0.93</v>
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>0.10000000000000003</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O20">
         <f t="shared" si="1"/>
-        <v>-8.0000000000000029E-2</v>
+        <v>0.91999999999999993</v>
       </c>
       <c r="P20">
         <f t="shared" si="1"/>
-        <v>0.10000000000000006</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q20">
         <f t="shared" si="1"/>
-        <v>9.9999999999999853E-2</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="R20">
-        <f t="shared" si="1"/>
-        <v>0.19999999999999996</v>
+        <f t="shared" si="0"/>
+        <v>1.2</v>
       </c>
       <c r="S20">
-        <f t="shared" si="1"/>
-        <v>0.10000000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T20">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
+        <f t="shared" si="0"/>
+        <v>1.3</v>
       </c>
       <c r="U20">
-        <f t="shared" si="1"/>
-        <v>0.35000000000000003</v>
+        <f t="shared" si="0"/>
+        <v>1.35</v>
       </c>
       <c r="V20">
-        <f t="shared" si="1"/>
-        <v>7.9999999999999988E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.08</v>
       </c>
       <c r="W20">
-        <f t="shared" si="1"/>
-        <v>6.9999999999999951E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0699999999999998</v>
       </c>
       <c r="X20">
-        <f t="shared" si="1"/>
-        <v>0.45000000000000012</v>
+        <f t="shared" si="0"/>
+        <v>1.4500000000000002</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="1"/>
-        <v>9.999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AB20">
         <f>AVERAGE(B20:Z20)</f>
-        <v>0.11160000000000002</v>
+        <v>1.1116000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.35">
@@ -2744,108 +2747,108 @@
         <v>3</v>
       </c>
       <c r="B21">
-        <f>(B6-B$3)/B$3</f>
-        <v>0.11999999999999988</v>
+        <f t="shared" si="1"/>
+        <v>1.1199999999999999</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:Z21" si="2">(C6-C$3)/C$3</f>
-        <v>0.10000000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000007</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
-        <v>0.11999999999999993</v>
+        <f t="shared" si="0"/>
+        <v>1.1199999999999999</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G21">
-        <f t="shared" si="2"/>
-        <v>0.1000000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
-        <v>0.35000000000000003</v>
+        <f t="shared" si="0"/>
+        <v>1.35</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
-        <v>9.9999999999999908E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="J21">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000012</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
-        <v>0.15000000000000002</v>
+        <f t="shared" si="0"/>
+        <v>1.1500000000000001</v>
       </c>
       <c r="L21">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000006</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M21">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000007</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N21">
-        <f t="shared" si="2"/>
-        <v>5.0000000000000017E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.05</v>
       </c>
       <c r="O21">
-        <f t="shared" si="2"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="P21">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000006</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="2"/>
-        <v>2.9999999999999957E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.03</v>
       </c>
       <c r="R21">
-        <f t="shared" si="2"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S21">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000031E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.01</v>
       </c>
       <c r="T21">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U21">
-        <f t="shared" si="2"/>
-        <v>2.0000000000000049E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.02</v>
       </c>
       <c r="V21">
-        <f t="shared" si="2"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="W21">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000002</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="X21">
-        <f t="shared" si="2"/>
-        <v>0.10000000000000014</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="2"/>
-        <v>0.20999999999999996</v>
+        <f t="shared" si="0"/>
+        <v>1.21</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="2"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AB21">
         <f>AVERAGE(B21:Z21)</f>
-        <v>0.10640000000000001</v>
+        <v>1.1064000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.35">
@@ -2853,108 +2856,108 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <f>(B7-B$3)/B$3</f>
-        <v>8.9999999999999969E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.0899999999999999</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:Z22" si="3">(C7-C$3)/C$3</f>
-        <v>0.10000000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000007</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
-        <v>4.9999999999999926E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0499999999999998</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
-        <v>3.0000000000000082E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.03</v>
       </c>
       <c r="H22">
-        <f t="shared" si="3"/>
-        <v>0.1000000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
-        <v>0.14999999999999997</v>
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000012</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
-        <v>0.21000000000000013</v>
+        <f t="shared" si="0"/>
+        <v>1.2100000000000002</v>
       </c>
       <c r="L22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000006</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M22">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000037E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.05</v>
       </c>
       <c r="N22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000003</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O22">
-        <f t="shared" si="3"/>
-        <v>6.9999999999999993E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.07</v>
       </c>
       <c r="P22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000006</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="3"/>
-        <v>7.9999999999999891E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0799999999999998</v>
       </c>
       <c r="R22">
-        <f t="shared" si="3"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T22">
-        <f t="shared" si="3"/>
-        <v>8.999999588407756E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0899999958840776</v>
       </c>
       <c r="U22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V22">
-        <f t="shared" si="3"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="W22">
-        <f t="shared" si="3"/>
-        <v>0.14999999999999997</v>
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
       </c>
       <c r="X22">
-        <f t="shared" si="3"/>
-        <v>0.10000000000000014</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="3"/>
-        <v>9.999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="3"/>
-        <v>0.12000000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
       </c>
       <c r="AB22">
         <f>AVERAGE(B22:Z22)</f>
-        <v>9.9599999835363148E-2</v>
+        <v>1.0995999998353634</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.35">
@@ -2970,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>29</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.35">
@@ -2978,107 +2981,107 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:Z26" si="4">(B4-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B26:Z26" si="2">(B4-B$3*$AD$19)/B$3</f>
         <v>9.9999999999999811E-2</v>
       </c>
       <c r="C26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="D26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000007</v>
       </c>
       <c r="E26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000002</v>
       </c>
       <c r="F26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.1000000000000001</v>
       </c>
       <c r="H26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.1000000000000001</v>
       </c>
       <c r="I26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.14999999999999997</v>
       </c>
       <c r="J26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000012</v>
       </c>
       <c r="K26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000013</v>
       </c>
       <c r="L26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="M26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>6.0000000000000081E-2</v>
       </c>
       <c r="N26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000003</v>
       </c>
       <c r="O26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="P26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>7.9999999999999891E-2</v>
       </c>
       <c r="R26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="S26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="T26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.25000002057961251</v>
       </c>
       <c r="U26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="V26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="W26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4.999999999999994E-2</v>
       </c>
       <c r="X26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.10000000000000014</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.999999999999995E-2</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="AB26" s="7">
-        <f t="shared" ref="AB26:AB37" si="5">AVERAGE(B26:Z26)</f>
+        <f t="shared" ref="AB26:AB37" si="3">AVERAGE(B26:Z26)</f>
         <v>0.10360000082318453</v>
       </c>
       <c r="AC26">
@@ -3091,111 +3094,111 @@
         <v>2</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:Z27" si="6">(B5-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B27:Z27" si="4">(B5-B$3*$AD$19)/B$3</f>
         <v>0.11999999999999988</v>
       </c>
       <c r="C27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="D27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.16000000000000011</v>
       </c>
       <c r="E27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.11999999999999993</v>
       </c>
       <c r="F27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="G27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.1000000000000001</v>
       </c>
       <c r="H27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>6.0000000000000026E-2</v>
       </c>
       <c r="I27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-2.0000000000000153E-2</v>
       </c>
       <c r="J27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.10000000000000012</v>
       </c>
       <c r="K27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-4.9999999999999906E-2</v>
       </c>
       <c r="L27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="M27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-6.9999999999999937E-2</v>
       </c>
       <c r="N27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.10000000000000003</v>
       </c>
       <c r="O27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-8.0000000000000029E-2</v>
       </c>
       <c r="P27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.9999999999999853E-2</v>
       </c>
       <c r="R27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="S27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="T27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
       <c r="U27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="V27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>7.9999999999999988E-2</v>
       </c>
       <c r="W27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>6.9999999999999951E-2</v>
       </c>
       <c r="X27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.45000000000000012</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.999999999999995E-2</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="AB27" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.11160000000000002</v>
       </c>
       <c r="AC27">
-        <f t="shared" ref="AC27:AC36" si="7">1+AB27</f>
+        <f t="shared" ref="AC27:AC36" si="5">1+AB27</f>
         <v>1.1115999999999999</v>
       </c>
     </row>
@@ -3204,111 +3207,111 @@
         <v>3</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:Z28" si="8">(B6-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B28:Z28" si="6">(B6-B$3*$AD$19)/B$3</f>
         <v>0.11999999999999988</v>
       </c>
       <c r="C28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="D28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000007</v>
       </c>
       <c r="E28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.11999999999999993</v>
       </c>
       <c r="F28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
       <c r="G28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.1000000000000001</v>
       </c>
       <c r="H28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="I28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.9999999999999908E-2</v>
       </c>
       <c r="J28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000012</v>
       </c>
       <c r="K28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="L28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="M28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000007</v>
       </c>
       <c r="N28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5.0000000000000017E-2</v>
       </c>
       <c r="O28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="P28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.9999999999999957E-2</v>
       </c>
       <c r="R28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="S28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000031E-2</v>
       </c>
       <c r="T28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
       <c r="U28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.0000000000000049E-2</v>
       </c>
       <c r="V28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="W28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000002</v>
       </c>
       <c r="X28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.10000000000000014</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="AB28" s="7">
+        <f t="shared" si="3"/>
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="AC28">
         <f t="shared" si="5"/>
-        <v>0.10640000000000001</v>
-      </c>
-      <c r="AC28">
-        <f t="shared" si="7"/>
         <v>1.1064000000000001</v>
       </c>
     </row>
@@ -3317,111 +3320,111 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <f t="shared" ref="B29:Z29" si="9">(B7-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B29:Z29" si="7">(B7-B$3*$AD$19)/B$3</f>
         <v>8.9999999999999969E-2</v>
       </c>
       <c r="C29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="D29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000007</v>
       </c>
       <c r="E29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4.9999999999999926E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="G29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3.0000000000000082E-2</v>
       </c>
       <c r="H29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.1000000000000001</v>
       </c>
       <c r="I29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.14999999999999997</v>
       </c>
       <c r="J29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000012</v>
       </c>
       <c r="K29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.21000000000000013</v>
       </c>
       <c r="L29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="M29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>5.0000000000000037E-2</v>
       </c>
       <c r="N29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000003</v>
       </c>
       <c r="O29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6.9999999999999993E-2</v>
       </c>
       <c r="P29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000006</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7.9999999999999891E-2</v>
       </c>
       <c r="R29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="S29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="T29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8.999999588407756E-2</v>
       </c>
       <c r="U29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000005</v>
       </c>
       <c r="V29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="W29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.14999999999999997</v>
       </c>
       <c r="X29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.10000000000000014</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.999999999999995E-2</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.12000000000000001</v>
       </c>
       <c r="AB29" s="7">
+        <f t="shared" si="3"/>
+        <v>9.9599999835363148E-2</v>
+      </c>
+      <c r="AC29">
         <f t="shared" si="5"/>
-        <v>9.9599999835363148E-2</v>
-      </c>
-      <c r="AC29">
-        <f t="shared" si="7"/>
         <v>1.0995999998353632</v>
       </c>
     </row>
@@ -3430,111 +3433,111 @@
         <v>5</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:Z30" si="10">(B8-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B30:Z30" si="8">(B8-B$3*$AD$19)/B$3</f>
         <v>-1.0000000000000037E-2</v>
       </c>
       <c r="C30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-0.10999999999999996</v>
       </c>
       <c r="D30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>5.0000000000000037E-2</v>
       </c>
       <c r="E30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-8.0000000000000113E-2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-9.9999999999999985E-3</v>
       </c>
       <c r="K30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-0.18999999999999995</v>
       </c>
       <c r="M30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-0.23000000000000007</v>
       </c>
       <c r="P30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-0.09</v>
       </c>
       <c r="R30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-1.0000000000000038E-2</v>
       </c>
       <c r="S30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-0.30000000000000004</v>
       </c>
       <c r="AB30" s="7">
+        <f t="shared" si="3"/>
+        <v>-3.9200000000000006E-2</v>
+      </c>
+      <c r="AC30">
         <f t="shared" si="5"/>
-        <v>-3.9200000000000006E-2</v>
-      </c>
-      <c r="AC30">
-        <f t="shared" si="7"/>
         <v>0.96079999999999999</v>
       </c>
     </row>
@@ -3543,111 +3546,111 @@
         <v>6</v>
       </c>
       <c r="B31">
-        <f t="shared" ref="B31:Z31" si="11">(B9-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B31:Z31" si="9">(B9-B$3*$AD$19)/B$3</f>
         <v>-0.22000000000000008</v>
       </c>
       <c r="C31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-1.0000000000000028E-2</v>
       </c>
       <c r="D31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.10999999999999989</v>
       </c>
       <c r="E31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4.9999999999999926E-2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-8.0000000000000029E-2</v>
       </c>
       <c r="G31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.25000000000000006</v>
       </c>
       <c r="J31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-4.9999999999999996E-2</v>
       </c>
       <c r="K31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-9.9999999999998875E-3</v>
       </c>
       <c r="L31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.10999999999999999</v>
       </c>
       <c r="M31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-7.9999999999999988E-2</v>
       </c>
       <c r="N31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.25</v>
       </c>
       <c r="P31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.21999999999999997</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.15000000000000002</v>
       </c>
       <c r="R31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-1.0000000000000031E-2</v>
       </c>
       <c r="T31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.24999999999999997</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB31" s="7">
+        <f t="shared" si="3"/>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="AC31">
         <f t="shared" si="5"/>
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="AC31">
-        <f t="shared" si="7"/>
         <v>0.92999999999999994</v>
       </c>
     </row>
@@ -3656,111 +3659,111 @@
         <v>7</v>
       </c>
       <c r="B32">
-        <f t="shared" ref="B32:Z32" si="12">(B10-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B32:Z32" si="10">(B10-B$3*$AD$19)/B$3</f>
         <v>-0.35000000000000009</v>
       </c>
       <c r="C32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.35000000000000003</v>
       </c>
       <c r="D32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-9.9999999999998215E-3</v>
       </c>
       <c r="E32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.10999999999999997</v>
       </c>
       <c r="F32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0.05</v>
       </c>
       <c r="G32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-7.9999999999999877E-2</v>
       </c>
       <c r="H32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.28000000000000003</v>
       </c>
       <c r="J32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.3</v>
       </c>
       <c r="K32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.35</v>
       </c>
       <c r="L32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-9.9999999999999152E-3</v>
       </c>
       <c r="M32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.10999999999999993</v>
       </c>
       <c r="N32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.16999999999999998</v>
       </c>
       <c r="O32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-5.0000000000000058E-2</v>
       </c>
       <c r="P32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.24999999999999994</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.21000000000000005</v>
       </c>
       <c r="R32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-1.0000004115922443E-2</v>
       </c>
       <c r="U32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="W32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="X32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-0.19999999999999998</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AB32" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.11160000016463691</v>
+      </c>
+      <c r="AC32">
         <f t="shared" si="5"/>
-        <v>-0.11160000016463691</v>
-      </c>
-      <c r="AC32">
-        <f t="shared" si="7"/>
         <v>0.88839999983536311</v>
       </c>
     </row>
@@ -3769,111 +3772,111 @@
         <v>8</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:Z33" si="13">(B11-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B33:Z33" si="11">(B11-B$3*$AD$19)/B$3</f>
         <v>-0.15</v>
       </c>
       <c r="C33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.22000000000000003</v>
       </c>
       <c r="D33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-4.999999999999985E-2</v>
       </c>
       <c r="E33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-9.9999999999999516E-3</v>
       </c>
       <c r="F33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.11000000000000006</v>
       </c>
       <c r="G33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5.0000000000000135E-2</v>
       </c>
       <c r="H33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-7.9999999999999974E-2</v>
       </c>
       <c r="I33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.21999999999999997</v>
       </c>
       <c r="J33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.20999999999999996</v>
       </c>
       <c r="K33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.25</v>
       </c>
       <c r="L33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5.00000000000001E-2</v>
       </c>
       <c r="M33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-1.0000000000000044E-2</v>
       </c>
       <c r="N33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.11</v>
       </c>
       <c r="O33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.16000000000000006</v>
       </c>
       <c r="P33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.2</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.25</v>
       </c>
       <c r="R33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.20000000000000007</v>
       </c>
       <c r="S33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-1.0000000000000024E-2</v>
       </c>
       <c r="V33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-0.15000000000000008</v>
       </c>
       <c r="X33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>2.9999999999999971E-2</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB33" s="7">
+        <f t="shared" si="3"/>
+        <v>-9.0400000000000008E-2</v>
+      </c>
+      <c r="AC33">
         <f t="shared" si="5"/>
-        <v>-9.0400000000000008E-2</v>
-      </c>
-      <c r="AC33">
-        <f t="shared" si="7"/>
         <v>0.90959999999999996</v>
       </c>
     </row>
@@ -3882,111 +3885,111 @@
         <v>9</v>
       </c>
       <c r="B34">
-        <f t="shared" ref="B34:Z34" si="14">(B12-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B34:Z34" si="12">(B12-B$3*$AD$19)/B$3</f>
         <v>-0.05</v>
       </c>
       <c r="C34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.25</v>
       </c>
       <c r="D34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.21999999999999989</v>
       </c>
       <c r="E34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.19000000000000009</v>
       </c>
       <c r="F34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-1.0000000000000054E-2</v>
       </c>
       <c r="G34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.10999999999999996</v>
       </c>
       <c r="H34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5.0000000000000051E-2</v>
       </c>
       <c r="I34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-8.0000000000000099E-2</v>
       </c>
       <c r="J34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.17999999999999997</v>
       </c>
       <c r="K34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.18999999999999989</v>
       </c>
       <c r="L34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.29999999999999993</v>
       </c>
       <c r="M34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-1.9999999999999903E-2</v>
       </c>
       <c r="N34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-9.999999999999969E-3</v>
       </c>
       <c r="O34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.11000000000000001</v>
       </c>
       <c r="P34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.15</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.29000000000000004</v>
       </c>
       <c r="R34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.15000000000000008</v>
       </c>
       <c r="S34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-0.18999999999999995</v>
       </c>
       <c r="T34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="V34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="W34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-9.0000000000000066E-2</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AB34" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.10559999999999997</v>
+      </c>
+      <c r="AC34">
         <f t="shared" si="5"/>
-        <v>-0.10559999999999997</v>
-      </c>
-      <c r="AC34">
-        <f t="shared" si="7"/>
         <v>0.89440000000000008</v>
       </c>
     </row>
@@ -3995,111 +3998,111 @@
         <v>10</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:Z35" si="15">(B13-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B35:Z35" si="13">(B13-B$3*$AD$19)/B$3</f>
         <v>-0.22000000000000008</v>
       </c>
       <c r="C35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.14999999999999997</v>
       </c>
       <c r="D35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.14999999999999994</v>
       </c>
       <c r="E35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.15000000000000011</v>
       </c>
       <c r="F35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.11000000000000006</v>
       </c>
       <c r="G35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-9.999999999999858E-3</v>
       </c>
       <c r="H35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.1099999999999999</v>
       </c>
       <c r="I35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4.9999999999999871E-2</v>
       </c>
       <c r="J35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-7.9999999999999988E-2</v>
       </c>
       <c r="K35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.10999999999999986</v>
       </c>
       <c r="L35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.24999999999999997</v>
       </c>
       <c r="M35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.25</v>
       </c>
       <c r="N35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.25999999999999995</v>
       </c>
       <c r="O35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-1.0000000000000038E-2</v>
       </c>
       <c r="P35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.10999999999999999</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.14000000000000004</v>
       </c>
       <c r="R35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="S35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>6.000000000000006E-2</v>
       </c>
       <c r="T35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-0.17999999176815495</v>
       </c>
       <c r="U35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-4.999999999999992E-2</v>
       </c>
       <c r="V35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="W35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-1.0000000000000064E-2</v>
       </c>
       <c r="X35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0.15</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AB35" s="7">
+        <f t="shared" si="3"/>
+        <v>-8.1599999670726217E-2</v>
+      </c>
+      <c r="AC35">
         <f t="shared" si="5"/>
-        <v>-8.1599999670726217E-2</v>
-      </c>
-      <c r="AC35">
-        <f t="shared" si="7"/>
         <v>0.91840000032927382</v>
       </c>
     </row>
@@ -4108,111 +4111,111 @@
         <v>11</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:Z36" si="16">(B14-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B36:Z36" si="14">(B14-B$3*$AD$19)/B$3</f>
         <v>-0.26000000000000006</v>
       </c>
       <c r="C36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.2599999999999999</v>
       </c>
       <c r="E36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.19000000000000009</v>
       </c>
       <c r="F36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.16000000000000006</v>
       </c>
       <c r="G36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.20999999999999988</v>
       </c>
       <c r="H36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-9.9999999999999759E-3</v>
       </c>
       <c r="I36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.10999999999999999</v>
       </c>
       <c r="J36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>5.0000000000000121E-2</v>
       </c>
       <c r="K36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-7.9999999999999877E-2</v>
       </c>
       <c r="L36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.2</v>
       </c>
       <c r="M36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.14999999999999994</v>
       </c>
       <c r="N36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.29999999999999993</v>
       </c>
       <c r="O36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.31000000000000011</v>
       </c>
       <c r="P36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-1.0000000000000028E-2</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.11000000000000008</v>
       </c>
       <c r="R36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.26000000000000006</v>
       </c>
       <c r="S36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>6.9999999999999951E-2</v>
       </c>
       <c r="T36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-4.0000016463689919E-2</v>
       </c>
       <c r="U36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-0.17</v>
       </c>
       <c r="V36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="W36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-9.9999999999999534E-3</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>-1.9999999999999931E-2</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB36" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.11280000065854759</v>
+      </c>
+      <c r="AC36">
         <f t="shared" si="5"/>
-        <v>-0.11280000065854759</v>
-      </c>
-      <c r="AC36">
-        <f t="shared" si="7"/>
         <v>0.88719999934145244</v>
       </c>
     </row>
@@ -4221,107 +4224,107 @@
         <v>12</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:H37" si="17">(B15-B$3*$AD$19)/B$3</f>
+        <f t="shared" ref="B37:H37" si="15">(B15-B$3*$AD$19)/B$3</f>
         <v>-0.29000000000000004</v>
       </c>
       <c r="C37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-1.0000000000000028E-2</v>
       </c>
       <c r="D37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-0.20999999999999996</v>
       </c>
       <c r="E37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-0.27</v>
       </c>
       <c r="F37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-0.19000000000000009</v>
       </c>
       <c r="G37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-0.16999999999999996</v>
       </c>
       <c r="H37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-7.9999999999999974E-2</v>
       </c>
       <c r="I37">
-        <f t="shared" ref="I37:Z37" si="18">(I15-I$3*$AD$19)/I$3</f>
+        <f t="shared" ref="I37:Z37" si="16">(I15-I$3*$AD$19)/I$3</f>
         <v>-1.0000000000000077E-2</v>
       </c>
       <c r="J37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-0.10999999999999999</v>
       </c>
       <c r="K37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>5.0000000000000065E-2</v>
       </c>
       <c r="L37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-4.9999999999999968E-2</v>
       </c>
       <c r="M37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-0.21000000000000002</v>
       </c>
       <c r="N37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-0.20000000000000009</v>
       </c>
       <c r="P37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-0.24999999999999994</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-9.9999999999999863E-3</v>
       </c>
       <c r="R37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-0.11000000000000001</v>
       </c>
       <c r="S37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-2.9999999999999961E-2</v>
       </c>
       <c r="T37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>7.9999991768155115E-2</v>
       </c>
       <c r="U37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="V37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-0.15999999999999998</v>
       </c>
       <c r="W37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>9.9999999999999378E-3</v>
       </c>
       <c r="X37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-1.9999999999999907E-2</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-1.000000000000004E-2</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AB37" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>-8.6400000329273807E-2</v>
       </c>
       <c r="AC37">
@@ -4373,103 +4376,103 @@
         <v>9.9999999999999811E-2</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:Z52" si="19">MIN(0.1,C26)</f>
+        <f t="shared" ref="C41:Z52" si="17">MIN(0.1,C26)</f>
         <v>0.1</v>
       </c>
       <c r="D41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="E41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="F41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="G41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="H41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="I41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="J41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="K41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="L41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="M41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>6.0000000000000081E-2</v>
       </c>
       <c r="N41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="O41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="P41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>7.9999999999999891E-2</v>
       </c>
       <c r="R41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="S41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="T41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="U41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="V41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="W41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>4.999999999999994E-2</v>
       </c>
       <c r="X41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>9.999999999999995E-2</v>
       </c>
       <c r="Z41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="AB41">
-        <f t="shared" ref="AB41:AB50" si="20">AVERAGE(B41:Z41)</f>
+        <f t="shared" ref="AB41:AB50" si="18">AVERAGE(B41:Z41)</f>
         <v>9.5600000000000004E-2</v>
       </c>
       <c r="AE41">
@@ -4477,7 +4480,7 @@
         <v>5.5999999999999994E-2</v>
       </c>
       <c r="AG41" s="7">
-        <f t="shared" ref="AG41:AG52" si="21">$AD$3 * AE41</f>
+        <f t="shared" ref="AG41:AG52" si="19">$AD$3 * AE41</f>
         <v>5.6</v>
       </c>
       <c r="AI41" s="9"/>
@@ -4487,115 +4490,115 @@
         <v>2</v>
       </c>
       <c r="B42">
-        <f t="shared" ref="B42:Q50" si="22">MIN(0.1,B27)</f>
+        <f t="shared" ref="B42:Q50" si="20">MIN(0.1,B27)</f>
         <v>0.1</v>
       </c>
       <c r="C42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="D42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="E42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="F42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="G42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="H42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>6.0000000000000026E-2</v>
       </c>
       <c r="I42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-2.0000000000000153E-2</v>
       </c>
       <c r="J42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="K42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-4.9999999999999906E-2</v>
       </c>
       <c r="L42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="M42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-6.9999999999999937E-2</v>
       </c>
       <c r="N42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="O42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-8.0000000000000029E-2</v>
       </c>
       <c r="P42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>9.9999999999999853E-2</v>
       </c>
       <c r="R42">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="17"/>
+        <v>7.9999999999999988E-2</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="17"/>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="17"/>
+        <v>9.999999999999995E-2</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="18"/>
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" ref="AE42:AE44" si="21">5.6%</f>
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="AG42" s="7">
         <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="S42">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="T42">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="U42">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="V42">
-        <f t="shared" si="19"/>
-        <v>7.9999999999999988E-2</v>
-      </c>
-      <c r="W42">
-        <f t="shared" si="19"/>
-        <v>6.9999999999999951E-2</v>
-      </c>
-      <c r="X42">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="Y42">
-        <f t="shared" si="19"/>
-        <v>9.999999999999995E-2</v>
-      </c>
-      <c r="Z42">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="AB42">
-        <f t="shared" si="20"/>
-        <v>7.1599999999999997E-2</v>
-      </c>
-      <c r="AE42">
-        <f t="shared" ref="AE42:AE44" si="23">5.6%</f>
-        <v>5.5999999999999994E-2</v>
-      </c>
-      <c r="AG42" s="7">
-        <f t="shared" si="21"/>
         <v>5.6</v>
       </c>
       <c r="AI42" s="8"/>
@@ -4605,115 +4608,115 @@
         <v>3</v>
       </c>
       <c r="B43">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.1</v>
       </c>
       <c r="C43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999908E-2</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000017E-2</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="17"/>
+        <v>2.9999999999999957E-2</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="17"/>
+        <v>1.0000000000000031E-2</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="17"/>
+        <v>2.0000000000000049E-2</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="AB43">
+        <f t="shared" si="18"/>
+        <v>8.840000000000002E-2</v>
+      </c>
+      <c r="AE43">
+        <f t="shared" si="21"/>
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="AG43" s="7">
         <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999908E-2</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="M43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="N43">
-        <f t="shared" si="19"/>
-        <v>5.0000000000000017E-2</v>
-      </c>
-      <c r="O43">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="Q43">
-        <f t="shared" si="19"/>
-        <v>2.9999999999999957E-2</v>
-      </c>
-      <c r="R43">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="S43">
-        <f t="shared" si="19"/>
-        <v>1.0000000000000031E-2</v>
-      </c>
-      <c r="T43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="U43">
-        <f t="shared" si="19"/>
-        <v>2.0000000000000049E-2</v>
-      </c>
-      <c r="V43">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="W43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="X43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="Y43">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="Z43">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="AB43">
-        <f t="shared" si="20"/>
-        <v>8.840000000000002E-2</v>
-      </c>
-      <c r="AE43">
-        <f t="shared" si="23"/>
-        <v>5.5999999999999994E-2</v>
-      </c>
-      <c r="AG43" s="7">
-        <f t="shared" si="21"/>
         <v>5.6</v>
       </c>
       <c r="AI43" s="9"/>
@@ -4723,115 +4726,115 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>8.9999999999999969E-2</v>
       </c>
       <c r="C44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="17"/>
+        <v>4.9999999999999926E-2</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="17"/>
+        <v>3.0000000000000082E-2</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000037E-2</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="17"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="17"/>
+        <v>7.9999999999999891E-2</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="17"/>
+        <v>8.999999588407756E-2</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="17"/>
+        <v>9.999999999999995E-2</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="18"/>
+        <v>9.0399999835363135E-2</v>
+      </c>
+      <c r="AE44">
+        <f t="shared" si="21"/>
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="AG44" s="7">
         <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="19"/>
-        <v>4.9999999999999926E-2</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="19"/>
-        <v>3.0000000000000082E-2</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="M44">
-        <f t="shared" si="19"/>
-        <v>5.0000000000000037E-2</v>
-      </c>
-      <c r="N44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="O44">
-        <f t="shared" si="19"/>
-        <v>6.9999999999999993E-2</v>
-      </c>
-      <c r="P44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="Q44">
-        <f t="shared" si="19"/>
-        <v>7.9999999999999891E-2</v>
-      </c>
-      <c r="R44">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="S44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="T44">
-        <f t="shared" si="19"/>
-        <v>8.999999588407756E-2</v>
-      </c>
-      <c r="U44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="V44">
-        <f t="shared" si="19"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="W44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="X44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="Y44">
-        <f t="shared" si="19"/>
-        <v>9.999999999999995E-2</v>
-      </c>
-      <c r="Z44">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="AB44">
-        <f t="shared" si="20"/>
-        <v>9.0399999835363135E-2</v>
-      </c>
-      <c r="AE44">
-        <f t="shared" si="23"/>
-        <v>5.5999999999999994E-2</v>
-      </c>
-      <c r="AG44" s="7">
-        <f t="shared" si="21"/>
         <v>5.6</v>
       </c>
       <c r="AI44" s="8"/>
@@ -4841,107 +4844,107 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-1.0000000000000037E-2</v>
       </c>
       <c r="C45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-0.10999999999999996</v>
       </c>
       <c r="D45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>5.0000000000000037E-2</v>
       </c>
       <c r="E45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-8.0000000000000113E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-9.9999999999999985E-3</v>
       </c>
       <c r="K45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-0.18999999999999995</v>
       </c>
       <c r="M45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-0.23000000000000007</v>
       </c>
       <c r="P45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-0.09</v>
       </c>
       <c r="R45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-1.0000000000000038E-2</v>
       </c>
       <c r="S45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="V45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="W45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Y45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Z45">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-0.30000000000000004</v>
       </c>
       <c r="AB45">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>-3.9200000000000006E-2</v>
       </c>
       <c r="AE45">
@@ -4949,7 +4952,7 @@
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="AG45" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>3.36</v>
       </c>
       <c r="AI45" s="9"/>
@@ -4959,115 +4962,115 @@
         <v>6</v>
       </c>
       <c r="B46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-0.22000000000000008</v>
       </c>
       <c r="C46">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000028E-2</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999989</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="17"/>
+        <v>4.9999999999999926E-2</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="17"/>
+        <v>-8.0000000000000029E-2</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="17"/>
+        <v>-0.25000000000000006</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="17"/>
+        <v>-4.9999999999999996E-2</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="17"/>
+        <v>-9.9999999999998875E-3</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999999</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="17"/>
+        <v>-7.9999999999999988E-2</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="17"/>
+        <v>-0.25</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="17"/>
+        <v>-0.21999999999999997</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="17"/>
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000031E-2</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="17"/>
+        <v>-0.24999999999999997</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AB46">
+        <f t="shared" si="18"/>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="AE46">
+        <f t="shared" ref="AE46:AE52" si="22">MAX(0.6*AG45/$AD$3, AB46)</f>
+        <v>2.0160000000000001E-2</v>
+      </c>
+      <c r="AG46" s="7">
         <f t="shared" si="19"/>
-        <v>-1.0000000000000028E-2</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999989</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="19"/>
-        <v>4.9999999999999926E-2</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="19"/>
-        <v>-8.0000000000000029E-2</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="19"/>
-        <v>-0.25000000000000006</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="19"/>
-        <v>-4.9999999999999996E-2</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="19"/>
-        <v>-9.9999999999998875E-3</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999999</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="19"/>
-        <v>-7.9999999999999988E-2</v>
-      </c>
-      <c r="N46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O46">
-        <f t="shared" si="19"/>
-        <v>-0.25</v>
-      </c>
-      <c r="P46">
-        <f t="shared" si="19"/>
-        <v>-0.21999999999999997</v>
-      </c>
-      <c r="Q46">
-        <f t="shared" si="19"/>
-        <v>-0.15000000000000002</v>
-      </c>
-      <c r="R46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="S46">
-        <f t="shared" si="19"/>
-        <v>-1.0000000000000031E-2</v>
-      </c>
-      <c r="T46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="U46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="V46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="W46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="X46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Y46">
-        <f t="shared" si="19"/>
-        <v>-0.24999999999999997</v>
-      </c>
-      <c r="Z46">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AB46">
-        <f t="shared" si="20"/>
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="AE46">
-        <f t="shared" ref="AE46:AE52" si="24">MAX(0.6*AG45/$AD$3, AB46)</f>
-        <v>2.0160000000000001E-2</v>
-      </c>
-      <c r="AG46" s="7">
-        <f t="shared" si="21"/>
         <v>2.016</v>
       </c>
       <c r="AI46" s="8"/>
@@ -5077,115 +5080,115 @@
         <v>7</v>
       </c>
       <c r="B47">
+        <f t="shared" si="20"/>
+        <v>-0.35000000000000009</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="17"/>
+        <v>-0.35000000000000003</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="17"/>
+        <v>-9.9999999999998215E-3</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999997</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="17"/>
+        <v>0.05</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="17"/>
+        <v>-7.9999999999999877E-2</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="17"/>
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="17"/>
+        <v>-0.3</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="17"/>
+        <v>-0.35</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="17"/>
+        <v>-9.9999999999999152E-3</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999993</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="17"/>
+        <v>-0.16999999999999998</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="17"/>
+        <v>-5.0000000000000058E-2</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="17"/>
+        <v>-0.24999999999999994</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="17"/>
+        <v>-0.21000000000000005</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="17"/>
+        <v>-1.0000004115922443E-2</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="17"/>
+        <v>-0.19999999999999998</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AB47">
+        <f t="shared" si="18"/>
+        <v>-0.11160000016463691</v>
+      </c>
+      <c r="AE47">
         <f t="shared" si="22"/>
-        <v>-0.35000000000000009</v>
-      </c>
-      <c r="C47">
+        <v>1.2096000000000001E-2</v>
+      </c>
+      <c r="AG47" s="7">
         <f t="shared" si="19"/>
-        <v>-0.35000000000000003</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="19"/>
-        <v>-9.9999999999998215E-3</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999997</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="19"/>
-        <v>0.05</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="19"/>
-        <v>-7.9999999999999877E-2</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="19"/>
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="19"/>
-        <v>-0.3</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="19"/>
-        <v>-0.35</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="19"/>
-        <v>-9.9999999999999152E-3</v>
-      </c>
-      <c r="M47">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999993</v>
-      </c>
-      <c r="N47">
-        <f t="shared" si="19"/>
-        <v>-0.16999999999999998</v>
-      </c>
-      <c r="O47">
-        <f t="shared" si="19"/>
-        <v>-5.0000000000000058E-2</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="19"/>
-        <v>-0.24999999999999994</v>
-      </c>
-      <c r="Q47">
-        <f t="shared" si="19"/>
-        <v>-0.21000000000000005</v>
-      </c>
-      <c r="R47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="S47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T47">
-        <f t="shared" si="19"/>
-        <v>-1.0000004115922443E-2</v>
-      </c>
-      <c r="U47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="V47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="W47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="X47">
-        <f t="shared" si="19"/>
-        <v>-0.19999999999999998</v>
-      </c>
-      <c r="Y47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Z47">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AB47">
-        <f t="shared" si="20"/>
-        <v>-0.11160000016463691</v>
-      </c>
-      <c r="AE47">
-        <f t="shared" si="24"/>
-        <v>1.2096000000000001E-2</v>
-      </c>
-      <c r="AG47" s="7">
-        <f t="shared" si="21"/>
         <v>1.2096</v>
       </c>
       <c r="AI47" s="9"/>
@@ -5195,115 +5198,115 @@
         <v>8</v>
       </c>
       <c r="B48">
+        <f t="shared" si="20"/>
+        <v>-0.15</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="17"/>
+        <v>-0.22000000000000003</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="17"/>
+        <v>-4.999999999999985E-2</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="17"/>
+        <v>-9.9999999999999516E-3</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="17"/>
+        <v>-0.11000000000000006</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000135E-2</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="17"/>
+        <v>-7.9999999999999974E-2</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="17"/>
+        <v>-0.21999999999999997</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="17"/>
+        <v>-0.20999999999999996</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="17"/>
+        <v>-0.25</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="17"/>
+        <v>5.00000000000001E-2</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000044E-2</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="17"/>
+        <v>-0.11</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="17"/>
+        <v>-0.16000000000000006</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="17"/>
+        <v>-0.2</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="17"/>
+        <v>-0.25</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="17"/>
+        <v>-0.20000000000000007</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000024E-2</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="17"/>
+        <v>-0.15000000000000008</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="17"/>
+        <v>2.9999999999999971E-2</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AB48">
+        <f t="shared" si="18"/>
+        <v>-9.0400000000000008E-2</v>
+      </c>
+      <c r="AE48">
         <f t="shared" si="22"/>
-        <v>-0.15</v>
-      </c>
-      <c r="C48">
+        <v>7.2575999999999995E-3</v>
+      </c>
+      <c r="AG48" s="7">
         <f t="shared" si="19"/>
-        <v>-0.22000000000000003</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="19"/>
-        <v>-4.999999999999985E-2</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="19"/>
-        <v>-9.9999999999999516E-3</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="19"/>
-        <v>-0.11000000000000006</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="19"/>
-        <v>5.0000000000000135E-2</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="19"/>
-        <v>-7.9999999999999974E-2</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="19"/>
-        <v>-0.21999999999999997</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="19"/>
-        <v>-0.20999999999999996</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="19"/>
-        <v>-0.25</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="19"/>
-        <v>5.00000000000001E-2</v>
-      </c>
-      <c r="M48">
-        <f t="shared" si="19"/>
-        <v>-1.0000000000000044E-2</v>
-      </c>
-      <c r="N48">
-        <f t="shared" si="19"/>
-        <v>-0.11</v>
-      </c>
-      <c r="O48">
-        <f t="shared" si="19"/>
-        <v>-0.16000000000000006</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="19"/>
-        <v>-0.2</v>
-      </c>
-      <c r="Q48">
-        <f t="shared" si="19"/>
-        <v>-0.25</v>
-      </c>
-      <c r="R48">
-        <f t="shared" si="19"/>
-        <v>-0.20000000000000007</v>
-      </c>
-      <c r="S48">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T48">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="U48">
-        <f t="shared" si="19"/>
-        <v>-1.0000000000000024E-2</v>
-      </c>
-      <c r="V48">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="W48">
-        <f t="shared" si="19"/>
-        <v>-0.15000000000000008</v>
-      </c>
-      <c r="X48">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Y48">
-        <f t="shared" si="19"/>
-        <v>2.9999999999999971E-2</v>
-      </c>
-      <c r="Z48">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AB48">
-        <f t="shared" si="20"/>
-        <v>-9.0400000000000008E-2</v>
-      </c>
-      <c r="AE48">
-        <f t="shared" si="24"/>
-        <v>7.2575999999999995E-3</v>
-      </c>
-      <c r="AG48" s="7">
-        <f t="shared" si="21"/>
         <v>0.72575999999999996</v>
       </c>
       <c r="AI48" s="8"/>
@@ -5313,115 +5316,115 @@
         <v>9</v>
       </c>
       <c r="B49">
+        <f t="shared" si="20"/>
+        <v>-0.05</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="17"/>
+        <v>-0.25</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="17"/>
+        <v>-0.21999999999999989</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="17"/>
+        <v>-0.19000000000000009</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000054E-2</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999996</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000051E-2</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="17"/>
+        <v>-8.0000000000000099E-2</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="17"/>
+        <v>-0.17999999999999997</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="17"/>
+        <v>-0.18999999999999989</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="17"/>
+        <v>-0.29999999999999993</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="17"/>
+        <v>-1.9999999999999903E-2</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="17"/>
+        <v>-9.999999999999969E-3</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="17"/>
+        <v>-0.11000000000000001</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="17"/>
+        <v>-0.15</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="17"/>
+        <v>-0.29000000000000004</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="17"/>
+        <v>-0.15000000000000008</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="17"/>
+        <v>-0.18999999999999995</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="17"/>
+        <v>-9.9999999999999978E-2</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="17"/>
+        <v>-9.0000000000000066E-2</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="18"/>
+        <v>-0.10559999999999997</v>
+      </c>
+      <c r="AE49">
         <f t="shared" si="22"/>
-        <v>-0.05</v>
-      </c>
-      <c r="C49">
+        <v>4.3545599999999995E-3</v>
+      </c>
+      <c r="AG49" s="7">
         <f t="shared" si="19"/>
-        <v>-0.25</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="19"/>
-        <v>-0.21999999999999989</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="19"/>
-        <v>-0.19000000000000009</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="19"/>
-        <v>-1.0000000000000054E-2</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999996</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="19"/>
-        <v>5.0000000000000051E-2</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="19"/>
-        <v>-8.0000000000000099E-2</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="19"/>
-        <v>-0.17999999999999997</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="19"/>
-        <v>-0.18999999999999989</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="19"/>
-        <v>-0.29999999999999993</v>
-      </c>
-      <c r="M49">
-        <f t="shared" si="19"/>
-        <v>-1.9999999999999903E-2</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="19"/>
-        <v>-9.999999999999969E-3</v>
-      </c>
-      <c r="O49">
-        <f t="shared" si="19"/>
-        <v>-0.11000000000000001</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="19"/>
-        <v>-0.15</v>
-      </c>
-      <c r="Q49">
-        <f t="shared" si="19"/>
-        <v>-0.29000000000000004</v>
-      </c>
-      <c r="R49">
-        <f t="shared" si="19"/>
-        <v>-0.15000000000000008</v>
-      </c>
-      <c r="S49">
-        <f t="shared" si="19"/>
-        <v>-0.18999999999999995</v>
-      </c>
-      <c r="T49">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="V49">
-        <f t="shared" si="19"/>
-        <v>-9.9999999999999978E-2</v>
-      </c>
-      <c r="W49">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="X49">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Y49">
-        <f t="shared" si="19"/>
-        <v>-9.0000000000000066E-2</v>
-      </c>
-      <c r="Z49">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AB49">
-        <f t="shared" si="20"/>
-        <v>-0.10559999999999997</v>
-      </c>
-      <c r="AE49">
-        <f t="shared" si="24"/>
-        <v>4.3545599999999995E-3</v>
-      </c>
-      <c r="AG49" s="7">
-        <f t="shared" si="21"/>
         <v>0.43545599999999995</v>
       </c>
       <c r="AI49" s="9"/>
@@ -5431,115 +5434,115 @@
         <v>10</v>
       </c>
       <c r="B50">
+        <f t="shared" si="20"/>
+        <v>-0.22000000000000008</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="17"/>
+        <v>-0.14999999999999997</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="17"/>
+        <v>-0.14999999999999994</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="17"/>
+        <v>-0.15000000000000011</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="17"/>
+        <v>-0.11000000000000006</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="17"/>
+        <v>-9.999999999999858E-3</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="17"/>
+        <v>-0.1099999999999999</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="17"/>
+        <v>4.9999999999999871E-2</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="17"/>
+        <v>-7.9999999999999988E-2</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999986</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="17"/>
+        <v>-0.24999999999999997</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="17"/>
+        <v>-0.25</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="17"/>
+        <v>-0.25999999999999995</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000038E-2</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999999</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="17"/>
+        <v>-0.14000000000000004</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="17"/>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="17"/>
+        <v>6.000000000000006E-2</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="17"/>
+        <v>-0.17999999176815495</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="17"/>
+        <v>-4.999999999999992E-2</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000064E-2</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AB50">
+        <f t="shared" si="18"/>
+        <v>-8.3599999670726219E-2</v>
+      </c>
+      <c r="AE50">
         <f t="shared" si="22"/>
-        <v>-0.22000000000000008</v>
-      </c>
-      <c r="C50">
+        <v>2.6127359999999992E-3</v>
+      </c>
+      <c r="AG50" s="7">
         <f t="shared" si="19"/>
-        <v>-0.14999999999999997</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="19"/>
-        <v>-0.14999999999999994</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="19"/>
-        <v>-0.15000000000000011</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="19"/>
-        <v>-0.11000000000000006</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="19"/>
-        <v>-9.999999999999858E-3</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="19"/>
-        <v>-0.1099999999999999</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="19"/>
-        <v>4.9999999999999871E-2</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="19"/>
-        <v>-7.9999999999999988E-2</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999986</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="19"/>
-        <v>-0.24999999999999997</v>
-      </c>
-      <c r="M50">
-        <f t="shared" si="19"/>
-        <v>-0.25</v>
-      </c>
-      <c r="N50">
-        <f t="shared" si="19"/>
-        <v>-0.25999999999999995</v>
-      </c>
-      <c r="O50">
-        <f t="shared" si="19"/>
-        <v>-1.0000000000000038E-2</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999999</v>
-      </c>
-      <c r="Q50">
-        <f t="shared" si="19"/>
-        <v>-0.14000000000000004</v>
-      </c>
-      <c r="R50">
-        <f t="shared" si="19"/>
-        <v>4.9999999999999989E-2</v>
-      </c>
-      <c r="S50">
-        <f t="shared" si="19"/>
-        <v>6.000000000000006E-2</v>
-      </c>
-      <c r="T50">
-        <f t="shared" si="19"/>
-        <v>-0.17999999176815495</v>
-      </c>
-      <c r="U50">
-        <f t="shared" si="19"/>
-        <v>-4.999999999999992E-2</v>
-      </c>
-      <c r="V50">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="W50">
-        <f t="shared" si="19"/>
-        <v>-1.0000000000000064E-2</v>
-      </c>
-      <c r="X50">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Y50">
-        <f t="shared" si="19"/>
-        <v>0.1</v>
-      </c>
-      <c r="Z50">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AB50">
-        <f t="shared" si="20"/>
-        <v>-8.3599999670726219E-2</v>
-      </c>
-      <c r="AE50">
-        <f t="shared" si="24"/>
-        <v>2.6127359999999992E-3</v>
-      </c>
-      <c r="AG50" s="7">
-        <f t="shared" si="21"/>
         <v>0.26127359999999994</v>
       </c>
       <c r="AI50" s="8"/>
@@ -5553,111 +5556,111 @@
         <v>-0.26000000000000006</v>
       </c>
       <c r="C51">
+        <f t="shared" si="17"/>
+        <v>-7.9999999999999988E-2</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="17"/>
+        <v>-0.2599999999999999</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="17"/>
+        <v>-0.19000000000000009</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="17"/>
+        <v>-0.16000000000000006</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="17"/>
+        <v>-0.20999999999999988</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="17"/>
+        <v>-9.9999999999999759E-3</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="17"/>
+        <v>-0.10999999999999999</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000121E-2</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="17"/>
+        <v>-7.9999999999999877E-2</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="17"/>
+        <v>-0.2</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="17"/>
+        <v>-0.14999999999999994</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="17"/>
+        <v>-0.29999999999999993</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="17"/>
+        <v>-0.31000000000000011</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000028E-2</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="17"/>
+        <v>-0.11000000000000008</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="17"/>
+        <v>-0.26000000000000006</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="17"/>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="17"/>
+        <v>-4.0000016463689919E-2</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="17"/>
+        <v>-0.17</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="17"/>
+        <v>-9.9999999999999534E-3</v>
+      </c>
+      <c r="Y51">
+        <f t="shared" si="17"/>
+        <v>-1.9999999999999931E-2</v>
+      </c>
+      <c r="Z51">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AB51">
+        <f t="shared" ref="AB51:AB52" si="23">AVERAGE(B51:Z51)</f>
+        <v>-0.11280000065854759</v>
+      </c>
+      <c r="AE51">
+        <f t="shared" si="22"/>
+        <v>1.5676415999999996E-3</v>
+      </c>
+      <c r="AG51" s="7">
         <f t="shared" si="19"/>
-        <v>-7.9999999999999988E-2</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="19"/>
-        <v>-0.2599999999999999</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="19"/>
-        <v>-0.19000000000000009</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="19"/>
-        <v>-0.16000000000000006</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="19"/>
-        <v>-0.20999999999999988</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="19"/>
-        <v>-9.9999999999999759E-3</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="19"/>
-        <v>-0.10999999999999999</v>
-      </c>
-      <c r="J51">
-        <f t="shared" si="19"/>
-        <v>5.0000000000000121E-2</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="19"/>
-        <v>-7.9999999999999877E-2</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="19"/>
-        <v>-0.2</v>
-      </c>
-      <c r="M51">
-        <f t="shared" si="19"/>
-        <v>-0.14999999999999994</v>
-      </c>
-      <c r="N51">
-        <f t="shared" si="19"/>
-        <v>-0.29999999999999993</v>
-      </c>
-      <c r="O51">
-        <f t="shared" si="19"/>
-        <v>-0.31000000000000011</v>
-      </c>
-      <c r="P51">
-        <f t="shared" si="19"/>
-        <v>-1.0000000000000028E-2</v>
-      </c>
-      <c r="Q51">
-        <f t="shared" si="19"/>
-        <v>-0.11000000000000008</v>
-      </c>
-      <c r="R51">
-        <f t="shared" si="19"/>
-        <v>-0.26000000000000006</v>
-      </c>
-      <c r="S51">
-        <f t="shared" si="19"/>
-        <v>6.9999999999999951E-2</v>
-      </c>
-      <c r="T51">
-        <f t="shared" si="19"/>
-        <v>-4.0000016463689919E-2</v>
-      </c>
-      <c r="U51">
-        <f t="shared" si="19"/>
-        <v>-0.17</v>
-      </c>
-      <c r="V51">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="W51">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="X51">
-        <f t="shared" si="19"/>
-        <v>-9.9999999999999534E-3</v>
-      </c>
-      <c r="Y51">
-        <f t="shared" si="19"/>
-        <v>-1.9999999999999931E-2</v>
-      </c>
-      <c r="Z51">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AB51">
-        <f t="shared" ref="AB51:AB52" si="25">AVERAGE(B51:Z51)</f>
-        <v>-0.11280000065854759</v>
-      </c>
-      <c r="AE51">
-        <f t="shared" si="24"/>
-        <v>1.5676415999999996E-3</v>
-      </c>
-      <c r="AG51" s="7">
-        <f t="shared" si="21"/>
         <v>0.15676415999999996</v>
       </c>
       <c r="AI51" s="9"/>
@@ -5671,111 +5674,111 @@
         <v>-0.29000000000000004</v>
       </c>
       <c r="C52">
+        <f t="shared" si="17"/>
+        <v>-1.0000000000000028E-2</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="17"/>
+        <v>-0.20999999999999996</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="17"/>
+        <v>-0.27</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="17"/>
+        <v>-0.19000000000000009</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="17"/>
+        <v>-0.16999999999999996</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="17"/>
+        <v>-7.9999999999999974E-2</v>
+      </c>
+      <c r="I52">
+        <f t="shared" ref="I52:Z52" si="24">MIN(0.1,I37)</f>
+        <v>-1.0000000000000077E-2</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="24"/>
+        <v>-0.10999999999999999</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="24"/>
+        <v>5.0000000000000065E-2</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="24"/>
+        <v>-4.9999999999999968E-2</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="24"/>
+        <v>-0.21000000000000002</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="24"/>
+        <v>-0.20000000000000009</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="24"/>
+        <v>-0.24999999999999994</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="24"/>
+        <v>-9.9999999999999863E-3</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="24"/>
+        <v>-0.11000000000000001</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="24"/>
+        <v>-2.9999999999999961E-2</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="24"/>
+        <v>7.9999991768155115E-2</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="24"/>
+        <v>9.0000000000000011E-2</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="24"/>
+        <v>-0.15999999999999998</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="24"/>
+        <v>9.9999999999999378E-3</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="24"/>
+        <v>-1.9999999999999907E-2</v>
+      </c>
+      <c r="Y52">
+        <f t="shared" si="24"/>
+        <v>-1.000000000000004E-2</v>
+      </c>
+      <c r="Z52">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AB52">
+        <f t="shared" si="23"/>
+        <v>-8.6400000329273807E-2</v>
+      </c>
+      <c r="AE52">
+        <f t="shared" si="22"/>
+        <v>9.405849599999998E-4</v>
+      </c>
+      <c r="AG52" s="7">
         <f t="shared" si="19"/>
-        <v>-1.0000000000000028E-2</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="19"/>
-        <v>-0.20999999999999996</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="19"/>
-        <v>-0.27</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="19"/>
-        <v>-0.19000000000000009</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="19"/>
-        <v>-0.16999999999999996</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="19"/>
-        <v>-7.9999999999999974E-2</v>
-      </c>
-      <c r="I52">
-        <f t="shared" ref="I52:Z52" si="26">MIN(0.1,I37)</f>
-        <v>-1.0000000000000077E-2</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="26"/>
-        <v>-0.10999999999999999</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="26"/>
-        <v>5.0000000000000065E-2</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="26"/>
-        <v>-4.9999999999999968E-2</v>
-      </c>
-      <c r="M52">
-        <f t="shared" si="26"/>
-        <v>-0.21000000000000002</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="O52">
-        <f t="shared" si="26"/>
-        <v>-0.20000000000000009</v>
-      </c>
-      <c r="P52">
-        <f t="shared" si="26"/>
-        <v>-0.24999999999999994</v>
-      </c>
-      <c r="Q52">
-        <f t="shared" si="26"/>
-        <v>-9.9999999999999863E-3</v>
-      </c>
-      <c r="R52">
-        <f t="shared" si="26"/>
-        <v>-0.11000000000000001</v>
-      </c>
-      <c r="S52">
-        <f t="shared" si="26"/>
-        <v>-2.9999999999999961E-2</v>
-      </c>
-      <c r="T52">
-        <f t="shared" si="26"/>
-        <v>7.9999991768155115E-2</v>
-      </c>
-      <c r="U52">
-        <f t="shared" si="26"/>
-        <v>9.0000000000000011E-2</v>
-      </c>
-      <c r="V52">
-        <f t="shared" si="26"/>
-        <v>-0.15999999999999998</v>
-      </c>
-      <c r="W52">
-        <f t="shared" si="26"/>
-        <v>9.9999999999999378E-3</v>
-      </c>
-      <c r="X52">
-        <f t="shared" si="26"/>
-        <v>-1.9999999999999907E-2</v>
-      </c>
-      <c r="Y52">
-        <f t="shared" si="26"/>
-        <v>-1.000000000000004E-2</v>
-      </c>
-      <c r="Z52">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="AB52">
-        <f t="shared" si="25"/>
-        <v>-8.6400000329273807E-2</v>
-      </c>
-      <c r="AE52">
-        <f t="shared" si="24"/>
-        <v>9.405849599999998E-4</v>
-      </c>
-      <c r="AG52" s="7">
-        <f t="shared" si="21"/>
         <v>9.4058495999999978E-2</v>
       </c>
       <c r="AI52" s="8"/>

</xml_diff>